<commit_message>
finished TrackerServiceC & recording test results
</commit_message>
<xml_diff>
--- a/Distributed Systems Tester Results.xlsx
+++ b/Distributed Systems Tester Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DMills\GC\Lab9.3-TrackerAPI\redundantFolder\lab-9-3-starter-ajabs226\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB76A448-728A-47BB-9509-DC0B55016B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1853A557-3593-49F7-A738-BE72FC6166C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6830" yWindow="5590" windowWidth="16200" windowHeight="9410" xr2:uid="{33C01718-69C5-45B4-B708-672427852A25}"/>
+    <workbookView xWindow="-7150" yWindow="930" windowWidth="16200" windowHeight="14100" xr2:uid="{33C01718-69C5-45B4-B708-672427852A25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Number of tokens</t>
   </si>
@@ -73,7 +73,7 @@
     <t>TrackerServiceC Test Results</t>
   </si>
   <si>
-    <t>ERRORS, won't run</t>
+    <t>TrackerServiceC - TrackerServiceA</t>
   </si>
 </sst>
 </file>
@@ -105,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,18 +158,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A676B73C-3500-414C-AF7A-26590FC4F65C}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,186 +501,186 @@
     <col min="2" max="5" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
-        <v>10000</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="4">
         <v>100000</v>
       </c>
-      <c r="D2" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="D2" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="4">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>26</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>26</v>
       </c>
-      <c r="D3" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E3" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3115</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>16616</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1802</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>24467</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>300</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>181</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>436</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>117</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>145</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>128</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>115</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>182</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>138</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>305</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>139</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>121</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>305</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>157</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>343</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>171</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>176</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>188</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>141</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>211</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>1069</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>1069</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -679,120 +688,393 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E15" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <v>6252</v>
+      </c>
+      <c r="C17" s="3">
+        <v>17962</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1942</v>
+      </c>
+      <c r="E17" s="3">
+        <v>21288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>322</v>
+      </c>
+      <c r="C18" s="3">
+        <v>143</v>
+      </c>
+      <c r="D18" s="3">
+        <v>201</v>
+      </c>
+      <c r="E18" s="3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>311</v>
+      </c>
+      <c r="C19" s="3">
+        <v>164</v>
+      </c>
+      <c r="D19" s="3">
+        <v>110</v>
+      </c>
+      <c r="E19" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3">
+        <v>303</v>
+      </c>
+      <c r="C20" s="3">
+        <v>147</v>
+      </c>
+      <c r="D20" s="3">
+        <v>155</v>
+      </c>
+      <c r="E20" s="3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3">
+        <v>251</v>
+      </c>
+      <c r="C21" s="3">
+        <v>149</v>
+      </c>
+      <c r="D21" s="3">
+        <v>105</v>
+      </c>
+      <c r="E21" s="3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3">
+        <v>304</v>
+      </c>
+      <c r="C22" s="3">
+        <v>179</v>
+      </c>
+      <c r="D22" s="3">
+        <v>835</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3">
+        <v>258</v>
+      </c>
+      <c r="C23" s="3">
+        <v>143</v>
+      </c>
+      <c r="D23" s="3">
+        <v>110</v>
+      </c>
+      <c r="E23" s="3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3">
+        <v>215</v>
+      </c>
+      <c r="C24" s="3">
+        <v>110</v>
+      </c>
+      <c r="D24" s="3">
+        <v>651</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="5">
-        <v>10000</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B28" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C28" s="4">
         <v>100000</v>
       </c>
-      <c r="D15" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="D28" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E28" s="4">
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B29" s="3">
         <v>26</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C29" s="3">
         <v>26</v>
       </c>
-      <c r="D16" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E16" s="5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="D29" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E29" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="B30" s="3">
+        <f>B17-B4</f>
+        <v>3137</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" ref="C30:E30" si="0">C17-C4</f>
+        <v>1346</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>-3179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="B31" s="3">
+        <f t="shared" ref="B31:E31" si="1">B18-B5</f>
+        <v>22</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="1"/>
+        <v>-38</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="1"/>
+        <v>-235</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>-163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="B32" s="3">
+        <f t="shared" ref="B32:E32" si="2">B19-B6</f>
+        <v>194</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="B33" s="3">
+        <f t="shared" ref="B33:E33" si="3">B20-B7</f>
+        <v>188</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="3"/>
+        <v>-35</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:E34" si="4">B21-B8</f>
+        <v>-54</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="4"/>
+        <v>-16</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="B35" s="3">
+        <f t="shared" ref="B35:E35" si="5">B22-B9</f>
+        <v>-1</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="5"/>
+        <v>492</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="5"/>
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="B36" s="3">
+        <f t="shared" ref="B36:E36" si="6">B23-B10</f>
+        <v>87</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="6"/>
+        <v>-33</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="6"/>
+        <v>-78</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="6"/>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="B37" s="3">
+        <f t="shared" ref="B37:E37" si="7">B24-B11</f>
+        <v>74</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="7"/>
+        <v>-101</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="7"/>
+        <v>-418</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>